<commit_message>
Making Sign Up Test Cases for another site
</commit_message>
<xml_diff>
--- a/target/test-classes/Data/UserData.xlsx
+++ b/target/test-classes/Data/UserData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="93">
   <si>
     <t>firstname</t>
   </si>
@@ -209,6 +209,96 @@
   </si>
   <si>
     <t>lilian.nikolaus@yahoo.com</t>
+  </si>
+  <si>
+    <t>mAlfonso</t>
+  </si>
+  <si>
+    <t>MDoyle</t>
+  </si>
+  <si>
+    <t>1-912-244-9624</t>
+  </si>
+  <si>
+    <t>watson.leuschke@hotmail.com</t>
+  </si>
+  <si>
+    <t>43043468MNon</t>
+  </si>
+  <si>
+    <t>MStanton</t>
+  </si>
+  <si>
+    <t>mWillms</t>
+  </si>
+  <si>
+    <t>violet.schuster@gmail.com</t>
+  </si>
+  <si>
+    <t>reinhold.mayer@gmail.com</t>
+  </si>
+  <si>
+    <t>layla.schuster@gmail.com</t>
+  </si>
+  <si>
+    <t>neoma.kassulke@yahoo.com</t>
+  </si>
+  <si>
+    <t>lurline.jacobson@hotmail.com</t>
+  </si>
+  <si>
+    <t>523049</t>
+  </si>
+  <si>
+    <t>claudine.hammes@hotmail.com</t>
+  </si>
+  <si>
+    <t>orie.bradtke@gmail.com</t>
+  </si>
+  <si>
+    <t>mSuzanne</t>
+  </si>
+  <si>
+    <t>MCronin</t>
+  </si>
+  <si>
+    <t>883-943-8971</t>
+  </si>
+  <si>
+    <t>orval.jakubowski@yahoo.com</t>
+  </si>
+  <si>
+    <t>13635568MNon</t>
+  </si>
+  <si>
+    <t>MNia</t>
+  </si>
+  <si>
+    <t>mCorwin</t>
+  </si>
+  <si>
+    <t>marcelo.tillman@hotmail.com</t>
+  </si>
+  <si>
+    <t>oren.kozey@yahoo.com</t>
+  </si>
+  <si>
+    <t>chase.adams@hotmail.com</t>
+  </si>
+  <si>
+    <t>hallie.ryan@hotmail.com</t>
+  </si>
+  <si>
+    <t>gaylord.reinger@yahoo.com</t>
+  </si>
+  <si>
+    <t>359433</t>
+  </si>
+  <si>
+    <t>bianka.legros@hotmail.com</t>
+  </si>
+  <si>
+    <t>letitia.cormier@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -527,7 +617,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -1160,6 +1250,406 @@
         <v>32</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" t="s">
+        <v>72</v>
+      </c>
+      <c r="E35" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" t="s">
+        <v>67</v>
+      </c>
+      <c r="F37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" t="s">
+        <v>75</v>
+      </c>
+      <c r="F38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" t="s">
+        <v>75</v>
+      </c>
+      <c r="F39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" t="s">
+        <v>77</v>
+      </c>
+      <c r="E41" t="s">
+        <v>67</v>
+      </c>
+      <c r="F41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" t="s">
+        <v>82</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" t="s">
+        <v>85</v>
+      </c>
+      <c r="E43" t="s">
+        <v>82</v>
+      </c>
+      <c r="F43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E44" t="s">
+        <v>82</v>
+      </c>
+      <c r="F44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" t="s">
+        <v>82</v>
+      </c>
+      <c r="F45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" t="s">
+        <v>88</v>
+      </c>
+      <c r="E46" t="s">
+        <v>82</v>
+      </c>
+      <c r="F46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" t="s">
+        <v>23</v>
+      </c>
+      <c r="E47" t="s">
+        <v>82</v>
+      </c>
+      <c r="F47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" t="s">
+        <v>89</v>
+      </c>
+      <c r="E48" t="s">
+        <v>90</v>
+      </c>
+      <c r="F48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E49" t="s">
+        <v>90</v>
+      </c>
+      <c r="F49" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" t="s">
+        <v>92</v>
+      </c>
+      <c r="E50" t="s">
+        <v>82</v>
+      </c>
+      <c r="F50" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" t="s">
+        <v>79</v>
+      </c>
+      <c r="C51" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" t="s">
+        <v>92</v>
+      </c>
+      <c r="E51" t="s">
+        <v>82</v>
+      </c>
+      <c r="F51" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>